<commit_message>
almost finished, made more refines, and more email functions.
</commit_message>
<xml_diff>
--- a/DigitalIsraelFund_System/App_Data/Excels/ניהול בקשות.xlsx
+++ b/DigitalIsraelFund_System/App_Data/Excels/ניהול בקשות.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>אחוז מענק</t>
   </si>
@@ -161,6 +161,27 @@
   </si>
   <si>
     <t>נחמן למד</t>
+  </si>
+  <si>
+    <t>intel</t>
+  </si>
+  <si>
+    <t>נקלט</t>
+  </si>
+  <si>
+    <t>מוטי</t>
+  </si>
+  <si>
+    <t>רווחה</t>
+  </si>
+  <si>
+    <t>טומי</t>
+  </si>
+  <si>
+    <t>amd</t>
+  </si>
+  <si>
+    <t>יחזקל</t>
   </si>
 </sst>
 </file>
@@ -628,11 +649,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,7 +664,7 @@
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
     <col min="8" max="8" width="25.5703125" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" customWidth="1"/>
     <col min="10" max="10" width="8.7109375" customWidth="1"/>
@@ -757,6 +778,52 @@
       </c>
       <c r="H5" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>57698</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6">
+        <v>55000</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>48726</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7">
+        <v>9999</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved alot of Table pages generic code to an App_Code page with helper functions
</commit_message>
<xml_diff>
--- a/DigitalIsraelFund_System/App_Data/Excels/ניהול בקשות.xlsx
+++ b/DigitalIsraelFund_System/App_Data/Excels/ניהול בקשות.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>אחוז מענק</t>
   </si>
@@ -182,6 +182,15 @@
   </si>
   <si>
     <t>יחזקל</t>
+  </si>
+  <si>
+    <t>microsoft</t>
+  </si>
+  <si>
+    <t>רומן</t>
+  </si>
+  <si>
+    <t>רותם גלבוע</t>
   </si>
 </sst>
 </file>
@@ -649,11 +658,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,6 +833,26 @@
       </c>
       <c r="H7" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>44888</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8">
+        <v>700000</v>
+      </c>
+      <c r="H8" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enabled the site to work with sql, improved the settings addition of a mashov.
</commit_message>
<xml_diff>
--- a/DigitalIsraelFund_System/App_Data/Excels/ניהול בקשות.xlsx
+++ b/DigitalIsraelFund_System/App_Data/Excels/ניהול בקשות.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
   <si>
     <t>אחוז מענק</t>
   </si>
@@ -136,9 +136,6 @@
     <t>תאור קצר של הפרויקט</t>
   </si>
   <si>
-    <t xml:space="preserve">גובה מענק שאושר </t>
-  </si>
-  <si>
     <t>בקשה אושרה כן/לא</t>
   </si>
   <si>
@@ -191,6 +188,30 @@
   </si>
   <si>
     <t>רותם גלבוע</t>
+  </si>
+  <si>
+    <t>בבדיקה</t>
+  </si>
+  <si>
+    <t>הוגשו חוו"ד</t>
+  </si>
+  <si>
+    <t>כן</t>
+  </si>
+  <si>
+    <t>אפליקציה לניטור פסיבי והתרעה מוקדמת על הופעת סיכון לשבץ מוחי</t>
+  </si>
+  <si>
+    <t>ניטור חדש של האינטרנט</t>
+  </si>
+  <si>
+    <t>לא</t>
+  </si>
+  <si>
+    <t>גובה מענק שאושר</t>
+  </si>
+  <si>
+    <t>22/3/15</t>
   </si>
 </sst>
 </file>
@@ -312,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -350,6 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,7 +684,7 @@
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +699,7 @@
     <col min="8" max="8" width="25.5703125" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" customWidth="1"/>
     <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
     <col min="12" max="12" width="8.28515625" customWidth="1"/>
     <col min="13" max="13" width="50.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.140625" customWidth="1"/>
@@ -685,7 +707,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -697,7 +719,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>4</v>
@@ -715,13 +737,13 @@
         <v>31</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>0</v>
@@ -740,7 +762,9 @@
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
@@ -754,7 +778,7 @@
         <v>8</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I4" s="16"/>
       <c r="J4" s="3">
@@ -769,24 +793,42 @@
       </c>
       <c r="N4" s="14"/>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>59782</v>
       </c>
       <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
         <v>42</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" t="s">
-        <v>43</v>
       </c>
       <c r="F5">
         <v>20000</v>
       </c>
       <c r="H5" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5">
+        <v>10000</v>
+      </c>
+      <c r="L5" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -794,22 +836,25 @@
         <v>57698</v>
       </c>
       <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>46</v>
-      </c>
-      <c r="D6" t="s">
-        <v>47</v>
       </c>
       <c r="F6">
         <v>55000</v>
       </c>
       <c r="G6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" t="s">
         <v>48</v>
       </c>
-      <c r="H6" t="s">
-        <v>49</v>
+      <c r="M6" s="15" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -817,13 +862,13 @@
         <v>48726</v>
       </c>
       <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
         <v>50</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s">
-        <v>51</v>
       </c>
       <c r="F7">
         <v>9999</v>
@@ -832,7 +877,7 @@
         <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -840,19 +885,22 @@
         <v>44888</v>
       </c>
       <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
         <v>52</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" t="s">
-        <v>53</v>
       </c>
       <c r="F8">
         <v>700000</v>
       </c>
       <c r="H8" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="J8" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>